<commit_message>
added HTML Report generation
</commit_message>
<xml_diff>
--- a/src/test/resources/OtherData/StockName.xlsx
+++ b/src/test/resources/OtherData/StockName.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="352">
   <si>
     <t>Stock Name</t>
   </si>
@@ -943,6 +943,141 @@
   </si>
   <si>
     <t>+24.25</t>
+  </si>
+  <si>
+    <t>26/05/2024</t>
+  </si>
+  <si>
+    <t>−33.75</t>
+  </si>
+  <si>
+    <t>−34.15</t>
+  </si>
+  <si>
+    <t>−2.45</t>
+  </si>
+  <si>
+    <t>+27.30</t>
+  </si>
+  <si>
+    <t>−7.15</t>
+  </si>
+  <si>
+    <t>−10.15</t>
+  </si>
+  <si>
+    <t>−40.20</t>
+  </si>
+  <si>
+    <t>+2.00</t>
+  </si>
+  <si>
+    <t>−15.75</t>
+  </si>
+  <si>
+    <t>−4.80</t>
+  </si>
+  <si>
+    <t>+35.60</t>
+  </si>
+  <si>
+    <t>−32.75</t>
+  </si>
+  <si>
+    <t>−13.10</t>
+  </si>
+  <si>
+    <t>−18.90</t>
+  </si>
+  <si>
+    <t>−0.60</t>
+  </si>
+  <si>
+    <t>−3.65</t>
+  </si>
+  <si>
+    <t>−0.050</t>
+  </si>
+  <si>
+    <t>−30.70</t>
+  </si>
+  <si>
+    <t>−41.05</t>
+  </si>
+  <si>
+    <t>−4.10</t>
+  </si>
+  <si>
+    <t>+3.55</t>
+  </si>
+  <si>
+    <t>+7.25</t>
+  </si>
+  <si>
+    <t>−7.05</t>
+  </si>
+  <si>
+    <t>−9.80</t>
+  </si>
+  <si>
+    <t>+2.15</t>
+  </si>
+  <si>
+    <t>−8.10</t>
+  </si>
+  <si>
+    <t>−10.95</t>
+  </si>
+  <si>
+    <t>+23.90</t>
+  </si>
+  <si>
+    <t>−42.50</t>
+  </si>
+  <si>
+    <t>−2.10</t>
+  </si>
+  <si>
+    <t>−0.85</t>
+  </si>
+  <si>
+    <t>+65.15</t>
+  </si>
+  <si>
+    <t>+2.70</t>
+  </si>
+  <si>
+    <t>+7.70</t>
+  </si>
+  <si>
+    <t>−11.05</t>
+  </si>
+  <si>
+    <t>−0.80</t>
+  </si>
+  <si>
+    <t>+2.20</t>
+  </si>
+  <si>
+    <t>+2.85</t>
+  </si>
+  <si>
+    <t>+15.45</t>
+  </si>
+  <si>
+    <t>−18.95</t>
+  </si>
+  <si>
+    <t>+12.70</t>
+  </si>
+  <si>
+    <t>−26.45</t>
+  </si>
+  <si>
+    <t>+67.40</t>
+  </si>
+  <si>
+    <t>+2.95</t>
   </si>
 </sst>
 </file>
@@ -1829,7 +1964,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -1848,6 +1983,9 @@
       <c r="B1" t="s" s="0">
         <v>259</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>307</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
@@ -1856,6 +1994,9 @@
       <c r="B2" t="s" s="0">
         <v>260</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>308</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
@@ -1864,6 +2005,9 @@
       <c r="B3" t="s" s="0">
         <v>261</v>
       </c>
+      <c r="C3" t="s" s="0">
+        <v>309</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
@@ -1872,6 +2016,9 @@
       <c r="B4" t="s" s="0">
         <v>262</v>
       </c>
+      <c r="C4" t="s" s="0">
+        <v>310</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
@@ -1880,6 +2027,9 @@
       <c r="B5" t="s" s="0">
         <v>263</v>
       </c>
+      <c r="C5" t="s" s="0">
+        <v>311</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s" s="0">
@@ -1888,6 +2038,9 @@
       <c r="B6" t="s" s="0">
         <v>264</v>
       </c>
+      <c r="C6" t="s" s="0">
+        <v>312</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s" s="0">
@@ -1896,6 +2049,9 @@
       <c r="B7" t="s" s="0">
         <v>265</v>
       </c>
+      <c r="C7" t="s" s="0">
+        <v>313</v>
+      </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s" s="0">
@@ -1904,6 +2060,9 @@
       <c r="B8" t="s" s="0">
         <v>266</v>
       </c>
+      <c r="C8" t="s" s="0">
+        <v>314</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s" s="0">
@@ -1912,6 +2071,9 @@
       <c r="B9" t="s" s="0">
         <v>267</v>
       </c>
+      <c r="C9" t="s" s="0">
+        <v>315</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s" s="0">
@@ -1920,6 +2082,9 @@
       <c r="B10" t="s" s="0">
         <v>268</v>
       </c>
+      <c r="C10" t="s" s="0">
+        <v>316</v>
+      </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s" s="0">
@@ -1928,6 +2093,9 @@
       <c r="B11" t="s" s="0">
         <v>269</v>
       </c>
+      <c r="C11" t="s" s="0">
+        <v>317</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s" s="0">
@@ -1936,6 +2104,9 @@
       <c r="B12" t="s" s="0">
         <v>270</v>
       </c>
+      <c r="C12" t="s" s="0">
+        <v>318</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s" s="0">
@@ -1944,6 +2115,9 @@
       <c r="B13" t="s" s="0">
         <v>271</v>
       </c>
+      <c r="C13" t="s" s="0">
+        <v>319</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s" s="0">
@@ -1952,6 +2126,9 @@
       <c r="B14" t="s" s="0">
         <v>266</v>
       </c>
+      <c r="C14" t="s" s="0">
+        <v>320</v>
+      </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s" s="0">
@@ -1960,6 +2137,9 @@
       <c r="B15" t="s" s="0">
         <v>272</v>
       </c>
+      <c r="C15" t="s" s="0">
+        <v>321</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s" s="0">
@@ -1968,6 +2148,9 @@
       <c r="B16" t="s" s="0">
         <v>273</v>
       </c>
+      <c r="C16" t="s" s="0">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s" s="0">
@@ -1976,6 +2159,9 @@
       <c r="B17" t="s" s="0">
         <v>274</v>
       </c>
+      <c r="C17" t="s" s="0">
+        <v>322</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s" s="0">
@@ -1984,6 +2170,9 @@
       <c r="B18" t="s" s="0">
         <v>275</v>
       </c>
+      <c r="C18" t="s" s="0">
+        <v>323</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s" s="0">
@@ -1992,6 +2181,9 @@
       <c r="B19" t="s" s="0">
         <v>276</v>
       </c>
+      <c r="C19" t="s" s="0">
+        <v>324</v>
+      </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s" s="0">
@@ -2000,6 +2192,9 @@
       <c r="B20" t="s" s="0">
         <v>277</v>
       </c>
+      <c r="C20" t="s" s="0">
+        <v>325</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s" s="0">
@@ -2008,6 +2203,9 @@
       <c r="B21" t="s" s="0">
         <v>278</v>
       </c>
+      <c r="C21" t="s" s="0">
+        <v>326</v>
+      </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s" s="0">
@@ -2016,6 +2214,9 @@
       <c r="B22" t="s" s="0">
         <v>279</v>
       </c>
+      <c r="C22" t="s" s="0">
+        <v>327</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s" s="0">
@@ -2024,6 +2225,9 @@
       <c r="B23" t="s" s="0">
         <v>280</v>
       </c>
+      <c r="C23" t="s" s="0">
+        <v>328</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s" s="0">
@@ -2032,6 +2236,9 @@
       <c r="B24" t="s" s="0">
         <v>281</v>
       </c>
+      <c r="C24" t="s" s="0">
+        <v>329</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s" s="0">
@@ -2040,6 +2247,9 @@
       <c r="B25" t="s" s="0">
         <v>282</v>
       </c>
+      <c r="C25" t="s" s="0">
+        <v>330</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s" s="0">
@@ -2048,6 +2258,9 @@
       <c r="B26" t="s" s="0">
         <v>283</v>
       </c>
+      <c r="C26" t="s" s="0">
+        <v>331</v>
+      </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s" s="0">
@@ -2056,6 +2269,9 @@
       <c r="B27" t="s" s="0">
         <v>284</v>
       </c>
+      <c r="C27" t="s" s="0">
+        <v>332</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s" s="0">
@@ -2064,6 +2280,9 @@
       <c r="B28" t="s" s="0">
         <v>285</v>
       </c>
+      <c r="C28" t="s" s="0">
+        <v>283</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s" s="0">
@@ -2072,6 +2291,9 @@
       <c r="B29" t="s" s="0">
         <v>286</v>
       </c>
+      <c r="C29" t="s" s="0">
+        <v>333</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s" s="0">
@@ -2080,6 +2302,9 @@
       <c r="B30" t="s" s="0">
         <v>287</v>
       </c>
+      <c r="C30" t="s" s="0">
+        <v>334</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s" s="0">
@@ -2088,6 +2313,9 @@
       <c r="B31" t="s" s="0">
         <v>288</v>
       </c>
+      <c r="C31" t="s" s="0">
+        <v>335</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s" s="0">
@@ -2096,6 +2324,9 @@
       <c r="B32" t="s" s="0">
         <v>289</v>
       </c>
+      <c r="C32" t="s" s="0">
+        <v>336</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s" s="0">
@@ -2104,6 +2335,9 @@
       <c r="B33" t="s" s="0">
         <v>290</v>
       </c>
+      <c r="C33" t="s" s="0">
+        <v>337</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s" s="0">
@@ -2112,6 +2346,9 @@
       <c r="B34" t="s" s="0">
         <v>291</v>
       </c>
+      <c r="C34" t="s" s="0">
+        <v>338</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s" s="0">
@@ -2120,6 +2357,9 @@
       <c r="B35" t="s" s="0">
         <v>292</v>
       </c>
+      <c r="C35" t="s" s="0">
+        <v>339</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s" s="0">
@@ -2128,6 +2368,9 @@
       <c r="B36" t="s" s="0">
         <v>293</v>
       </c>
+      <c r="C36" t="s" s="0">
+        <v>340</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s" s="0">
@@ -2136,6 +2379,9 @@
       <c r="B37" t="s" s="0">
         <v>294</v>
       </c>
+      <c r="C37" t="s" s="0">
+        <v>341</v>
+      </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s" s="0">
@@ -2144,6 +2390,9 @@
       <c r="B38" t="s" s="0">
         <v>295</v>
       </c>
+      <c r="C38" t="s" s="0">
+        <v>342</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s" s="0">
@@ -2152,6 +2401,9 @@
       <c r="B39" t="s" s="0">
         <v>296</v>
       </c>
+      <c r="C39" t="s" s="0">
+        <v>343</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s" s="0">
@@ -2160,6 +2412,9 @@
       <c r="B40" t="s" s="0">
         <v>77</v>
       </c>
+      <c r="C40" t="s" s="0">
+        <v>344</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s" s="0">
@@ -2168,6 +2423,9 @@
       <c r="B41" t="s" s="0">
         <v>297</v>
       </c>
+      <c r="C41" t="s" s="0">
+        <v>345</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s" s="0">
@@ -2176,6 +2434,9 @@
       <c r="B42" t="s" s="0">
         <v>298</v>
       </c>
+      <c r="C42" t="s" s="0">
+        <v>346</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s" s="0">
@@ -2184,6 +2445,9 @@
       <c r="B43" t="s" s="0">
         <v>299</v>
       </c>
+      <c r="C43" t="s" s="0">
+        <v>347</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s" s="0">
@@ -2192,6 +2456,9 @@
       <c r="B44" t="s" s="0">
         <v>300</v>
       </c>
+      <c r="C44" t="s" s="0">
+        <v>348</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s" s="0">
@@ -2200,6 +2467,9 @@
       <c r="B45" t="s" s="0">
         <v>301</v>
       </c>
+      <c r="C45" t="s" s="0">
+        <v>54</v>
+      </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s" s="0">
@@ -2208,6 +2478,9 @@
       <c r="B46" t="s" s="0">
         <v>302</v>
       </c>
+      <c r="C46" t="s" s="0">
+        <v>349</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s" s="0">
@@ -2216,6 +2489,9 @@
       <c r="B47" t="s" s="0">
         <v>285</v>
       </c>
+      <c r="C47" t="s" s="0">
+        <v>294</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s" s="0">
@@ -2224,6 +2500,9 @@
       <c r="B48" t="s" s="0">
         <v>303</v>
       </c>
+      <c r="C48" t="s" s="0">
+        <v>331</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s" s="0">
@@ -2232,6 +2511,9 @@
       <c r="B49" t="s" s="0">
         <v>304</v>
       </c>
+      <c r="C49" t="s" s="0">
+        <v>350</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s" s="0">
@@ -2240,6 +2522,9 @@
       <c r="B50" t="s" s="0">
         <v>305</v>
       </c>
+      <c r="C50" t="s" s="0">
+        <v>351</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s" s="0">
@@ -2247,6 +2532,9 @@
       </c>
       <c r="B51" t="s" s="0">
         <v>306</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>